<commit_message>
feat: update test file
</commit_message>
<xml_diff>
--- a/documents/BDP305x_TestCases_template.xlsx
+++ b/documents/BDP305x_TestCases_template.xlsx
@@ -14,8 +14,8 @@
     <sheet name="Test Report" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Admin!$A$8:$I$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Participant!$A$8:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Admin!$A$8:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Participant!$A$8:$I$13</definedName>
     <definedName name="ACTION">#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166">
   <si>
     <t>Template</t>
   </si>
@@ -185,13 +185,19 @@
     <t>5</t>
   </si>
   <si>
+    <t>Set final price for session</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Get User List</t>
   </si>
   <si>
     <t>Get user list</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Get User Info</t>
@@ -203,7 +209,7 @@
     <t>User address is existed</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Update User Info</t>
@@ -212,15 +218,12 @@
     <t>Update only email and name</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Set final price for session</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>Sign in</t>
   </si>
   <si>
@@ -230,7 +233,7 @@
     <t>Sign in into application</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>Sign up</t>
@@ -239,10 +242,10 @@
     <t>Sign up new account</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Submit Price</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Submit propose price</t>
   </si>
   <si>
     <t>Submit pricing for a product session</t>
@@ -260,7 +263,7 @@
     <t>Test requirement</t>
   </si>
   <si>
-    <t>&lt;Brief description about requirements which are tested in this sheet&gt;</t>
+    <t>User is admin/author of smart contract</t>
   </si>
   <si>
     <t>Fail</t>
@@ -308,126 +311,289 @@
     <t>Note</t>
   </si>
   <si>
-    <t>A Sample Function</t>
-  </si>
-  <si>
-    <t>Sample case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">&lt;Brief description of this case: what is tested?&gt;
+    <t>Admin-1.1</t>
+  </si>
+  <si>
+    <t>Init a session with name, description, images and timeout</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. At session page, click Add new session button
+3. Fullfil name, description, images and timeout of session
+4. Click Crease session button
+5. Confirm on Metamask</t>
+  </si>
+  <si>
+    <t>1. New session will be added in blockchain network.
+2. Admin will be redirected to session list, with display new session in the table</t>
+  </si>
+  <si>
+    <t>New session is added and display in session list</t>
+  </si>
+  <si>
+    <t>Get session list</t>
+  </si>
+  <si>
+    <t>Admin-2.1</t>
+  </si>
+  <si>
+    <t>Get session list as table when access to session page</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access homepage (session page)</t>
+  </si>
+  <si>
+    <t>A Table with Session list will be display</t>
+  </si>
+  <si>
+    <t>A Table with Session list is display</t>
+  </si>
+  <si>
+    <t>Get session detail</t>
+  </si>
+  <si>
+    <t>Admin-3.1</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access homepage (session page)
+3. Click view detail of one session</t>
+  </si>
+  <si>
+    <t>Session info will be display: name, description, images, status, propose price, final price</t>
+  </si>
+  <si>
+    <t>A session need to be created before</t>
+  </si>
+  <si>
+    <t>Session info is display: name, description, images, status, propose price, final price</t>
+  </si>
+  <si>
+    <t>Close Pricing session</t>
+  </si>
+  <si>
+    <t>2. Access homepage (sessioin page)</t>
+  </si>
+  <si>
+    <t>Admin-4.1</t>
+  </si>
+  <si>
+    <t>Close a ongoing session</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access homepage (session page)
+3. Click view detail of one session
+4. Click close session button</t>
+  </si>
+  <si>
+    <t>1. That session will be closed.
+2. Propose price for that session will be calculated and udpated.
+3. Admin will be redirected to session list</t>
+  </si>
+  <si>
+    <t>That session is closed, status is updated in session list. Moreover, proposed price is updated</t>
+  </si>
+  <si>
+    <t>Set Pricing session final price</t>
+  </si>
+  <si>
+    <t>Admin-5.1</t>
+  </si>
+  <si>
+    <t>Set final price for a closed session</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access homepage (session page)
+3. Click view detail of one session that is closed
+4. Enter final price and click Set final price button</t>
+  </si>
+  <si>
+    <t>1. FInal price of that session will be updated
+2. Admin can only set final price only one
+3. Deviation of all user that propose that session will be updated
+4. Admin will be redirected to session list</t>
+  </si>
+  <si>
+    <t>That session need to be created and closed, and have not been set final price</t>
+  </si>
+  <si>
+    <t>Final price of that session is updated. Deviation of all related user are updated, but not correct.</t>
+  </si>
+  <si>
+    <t>Get participant list</t>
+  </si>
+  <si>
+    <t>Admin-6.1</t>
+  </si>
+  <si>
+    <t>Get participant list as table when access to session page</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access participant page through header</t>
+  </si>
+  <si>
+    <t>A Table with Participant list will be display</t>
+  </si>
+  <si>
+    <t>A Table with Participant list is display</t>
+  </si>
+  <si>
+    <t>Get participant info</t>
+  </si>
+  <si>
+    <t>Admin-7.1</t>
+  </si>
+  <si>
+    <t>Get one participant detail info</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access participant page
+3. Click view one participant in the list</t>
+  </si>
+  <si>
+    <t>Detail of participant will be display, with email, name, deviation and session count</t>
+  </si>
+  <si>
+    <t>Detail of participant is display, with email, name, deviation and session count</t>
+  </si>
+  <si>
+    <t>Update participant info</t>
+  </si>
+  <si>
+    <t>Admin-8.1</t>
+  </si>
+  <si>
+    <t>Update one participant email and name</t>
+  </si>
+  <si>
+    <t>1. Access the system with Admin role, with Metamask extension in browser.
+2. Access participant page
+3. Click view one participant in the list
+4. Edit email and name, then click Edit button</t>
+  </si>
+  <si>
+    <t>That participant email and name will be updated.
+Admin will be redirected to participant list page, then see new info of participant</t>
+  </si>
+  <si>
+    <t>Email and name of participant are updated</t>
+  </si>
+  <si>
+    <t>Participant Functions</t>
+  </si>
+  <si>
+    <t>User is participant of application, and is not admin</t>
+  </si>
+  <si>
+    <t>Participant-1.1</t>
+  </si>
+  <si>
+    <t>1. Access the system with Participant role, with Metamask extension in browser.
+2. Access homepage (session page)</t>
+  </si>
+  <si>
+    <t>Need to sign in successfully</t>
+  </si>
+  <si>
+    <t>Participant-2.1</t>
+  </si>
+  <si>
+    <t>1. Access the system with Participant role, with Metamask extension in browser.
+2. Access homepage (session page)
+3. Click view detail of one session</t>
+  </si>
+  <si>
+    <t>Session info will be display: name, description, images, status, final price</t>
+  </si>
+  <si>
+    <t>Session info is display: name, description, images, status, final price</t>
+  </si>
+  <si>
+    <t>Participant-3.1</t>
+  </si>
+  <si>
+    <t>Get current participant detail info</t>
+  </si>
+  <si>
+    <t>1. Access the system with Participant role, with Metamask extension in browser.
+2. Access user info page</t>
+  </si>
+  <si>
+    <t>Detail of participancurrent t will be display, with email, name, deviation and session count</t>
+  </si>
+  <si>
+    <t>Detail of current participant is display, with email, name, deviation and session count</t>
+  </si>
+  <si>
+    <t>Update user info</t>
+  </si>
+  <si>
+    <t>Participant-4.1</t>
+  </si>
+  <si>
+    <t>1. Access the system with Participant role, with Metamask extension in browser.
+2. Access user info page
+3. Edit email and name, then click Edit button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That participant email and name will be updated.
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Ex: Test viewing "Company" form.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">&lt;Describe steps to perform this case&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Ex:
-1. Login the system with Manager role.
-2. Click "Company" tab in the left menu.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">&lt;Describe results which meet customer's requirement&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Ex:
-The "Company" view form is displayed with the following information:
-- Company name
-- Company address
-- Phone
-- Fax</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;List all test cases or conditions that must be done before performing this case&gt;
-</t>
-  </si>
-  <si>
-    <t>&lt;Describe actual result of the test&gt;</t>
-  </si>
-  <si>
-    <t>Admin-1.1</t>
-  </si>
-  <si>
-    <t>&lt;Test case 1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Function name&gt;</t>
-  </si>
-  <si>
-    <t>Admin-2.1</t>
-  </si>
-  <si>
-    <t>&lt;Test case 2&gt;</t>
-  </si>
-  <si>
-    <t>Admin-2.2</t>
-  </si>
-  <si>
-    <t>&lt;Test case 3&gt;</t>
-  </si>
-  <si>
-    <t>Participant Functions</t>
-  </si>
-  <si>
-    <t>&lt;ID of the requirement which are tested in this sheet&gt;</t>
-  </si>
-  <si>
-    <t>Update Participant Info</t>
-  </si>
-  <si>
-    <t>Participant-1.1</t>
-  </si>
-  <si>
-    <t>Update Participant Fullname and Email</t>
-  </si>
-  <si>
-    <t>&lt;Test case 4&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Test case 5&gt;</t>
+  </si>
+  <si>
+    <t>Participant-5.1</t>
+  </si>
+  <si>
+    <t>1. Access login page.
+2. Click login with Metamask</t>
+  </si>
+  <si>
+    <t>User will be redirect to homepage if success, else redirected to sign up/register page</t>
+  </si>
+  <si>
+    <t>User is redirect to homepage if success, else redirected to sign up/register page</t>
+  </si>
+  <si>
+    <t>Participant-6.1</t>
+  </si>
+  <si>
+    <t>Sign up/Register new account</t>
+  </si>
+  <si>
+    <t>1. Access login page.
+2. Click login with Metamask
+3. Enter email and name, then click Register  button</t>
+  </si>
+  <si>
+    <t>Participant will be added, then redirect to session list page</t>
+  </si>
+  <si>
+    <t>User is not signup</t>
+  </si>
+  <si>
+    <t>Participant is added, then redirect to session list page</t>
+  </si>
+  <si>
+    <t>Participant-7.1</t>
+  </si>
+  <si>
+    <t>Submit propose price for one session</t>
+  </si>
+  <si>
+    <t>1. Access the system with Participant role, with Metamask extension in browser.
+2. Access homepage (session page)
+3. Click view detail of one session
+4. Enter price then click Submit Price button</t>
+  </si>
+  <si>
+    <t>Propose price of participant will be submited and stored for that session</t>
+  </si>
+  <si>
+    <t>Propose price of participant is submited and stored for that session</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -539,13 +705,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
@@ -1515,7 +1681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1587,9 +1753,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1620,15 +1784,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1641,12 +1796,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="1" fillId="2" borderId="1" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1655,20 +1805,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1676,20 +1822,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2248,472 +2388,472 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.90789473684211" style="93" customWidth="1"/>
-    <col min="2" max="8" width="8.26973684210526" style="93" customWidth="1"/>
-    <col min="9" max="10" width="14.3618421052632" style="93" customWidth="1"/>
-    <col min="11" max="13" width="8.26973684210526" style="93" customWidth="1"/>
-    <col min="14" max="14" width="8.63157894736842" style="93" customWidth="1"/>
-    <col min="15" max="15" width="7.26973684210526" style="93" customWidth="1"/>
-    <col min="16" max="16" width="4.36184210526316" style="93" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="93"/>
+    <col min="1" max="1" width="1.90789473684211" style="83" customWidth="1"/>
+    <col min="2" max="8" width="8.26973684210526" style="83" customWidth="1"/>
+    <col min="9" max="10" width="14.3618421052632" style="83" customWidth="1"/>
+    <col min="11" max="13" width="8.26973684210526" style="83" customWidth="1"/>
+    <col min="14" max="14" width="8.63157894736842" style="83" customWidth="1"/>
+    <col min="15" max="15" width="7.26973684210526" style="83" customWidth="1"/>
+    <col min="16" max="16" width="4.36184210526316" style="83" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="83"/>
   </cols>
   <sheetData>
     <row r="2" ht="12.8" spans="2:15">
-      <c r="B2" s="94"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="119"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="109"/>
     </row>
     <row r="3" ht="12.8" spans="2:15">
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="120"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="110"/>
     </row>
     <row r="4" ht="16.4" spans="2:15">
-      <c r="B4" s="97"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="120"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="110"/>
     </row>
     <row r="5" ht="16.4" spans="2:15">
-      <c r="B5" s="97"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="120"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="110"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="120"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="110"/>
     </row>
     <row r="7" ht="12.8" spans="2:15">
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="120"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="110"/>
     </row>
     <row r="8" ht="12.8" spans="2:15">
-      <c r="B8" s="97"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="120"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="110"/>
     </row>
     <row r="9" ht="21.2" spans="2:15">
-      <c r="B9" s="97"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="120"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="110"/>
     </row>
     <row r="10" ht="38.5" customHeight="1" spans="2:15">
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="103"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="121"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="111"/>
     </row>
     <row r="11" ht="37" customHeight="1" spans="2:15">
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="121"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="111"/>
     </row>
     <row r="12" ht="27.6" spans="2:15">
-      <c r="B12" s="104"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="105"/>
-      <c r="N12" s="105"/>
-      <c r="O12" s="122"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="95"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="112"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="97"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="120"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="110"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="97"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="120"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="110"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="97"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="111" t="s">
+      <c r="B15" s="87"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="117" t="s">
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="117"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="120"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="110"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="113" t="s">
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="118" t="s">
+      <c r="G16" s="104"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="118"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="120"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="110"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="97"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="98"/>
-      <c r="N17" s="98"/>
-      <c r="O17" s="120"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="88"/>
+      <c r="O17" s="110"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="97"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="120"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
+      <c r="O18" s="110"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="97"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="120"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="110"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="97"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="98"/>
-      <c r="N20" s="98"/>
-      <c r="O20" s="120"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
+      <c r="O20" s="110"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="97"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="120"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="110"/>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="97"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="98"/>
-      <c r="N22" s="98"/>
-      <c r="O22" s="120"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
+      <c r="O22" s="110"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="97"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="115"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
-      <c r="N23" s="98"/>
-      <c r="O23" s="120"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
+      <c r="O23" s="110"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="108"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
-      <c r="O24" s="123"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="113"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="98"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="98"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="98"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="98"/>
-      <c r="J29" s="98"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="88"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="88"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="98"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="105"/>
+      <c r="F30" s="105"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="98"/>
-      <c r="J31" s="98"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2738,270 +2878,285 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="1.36184210526316" style="72" customWidth="1"/>
-    <col min="2" max="2" width="5.90789473684211" style="72" customWidth="1"/>
-    <col min="3" max="3" width="23.7236842105263" style="73" customWidth="1"/>
-    <col min="4" max="4" width="17.0921052631579" style="73" customWidth="1"/>
-    <col min="5" max="5" width="49.6315789473684" style="73" customWidth="1"/>
-    <col min="6" max="6" width="30.6315789473684" style="73" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="72"/>
+    <col min="1" max="1" width="1.36184210526316" style="62" customWidth="1"/>
+    <col min="2" max="2" width="5.90789473684211" style="62" customWidth="1"/>
+    <col min="3" max="3" width="23.7236842105263" style="63" customWidth="1"/>
+    <col min="4" max="4" width="17.0921052631579" style="63" customWidth="1"/>
+    <col min="5" max="5" width="49.6315789473684" style="63" customWidth="1"/>
+    <col min="6" max="6" width="30.6315789473684" style="63" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="62"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.2" spans="1:6">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="2:5">
-      <c r="B2" s="75"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="B2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-    </row>
-    <row r="4" s="69" customFormat="1" ht="84.75" customHeight="1" spans="2:6">
-      <c r="B4" s="79" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+    </row>
+    <row r="4" s="59" customFormat="1" ht="84.75" customHeight="1" spans="2:6">
+      <c r="B4" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="81"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-    </row>
-    <row r="6" s="70" customFormat="1" spans="2:6">
-      <c r="B6" s="83"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-    </row>
-    <row r="7" s="71" customFormat="1" ht="21" customHeight="1" spans="2:6">
-      <c r="B7" s="85" t="s">
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" s="60" customFormat="1" spans="2:6">
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+    </row>
+    <row r="7" s="61" customFormat="1" ht="21" customHeight="1" spans="2:6">
+      <c r="B7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="82" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="87">
+      <c r="B8" s="77">
         <v>1</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="88" t="s">
+      <c r="E8" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="78" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="88" t="s">
+      <c r="E9" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="88"/>
+      <c r="F9" s="78"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="88" t="s">
+      <c r="E10" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="88" t="s">
+      <c r="F10" s="78" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="78" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="87" t="s">
+    <row r="12" s="62" customFormat="1" spans="2:6">
+      <c r="B12" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="88" t="s">
+      <c r="D12" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="78"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="88"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="87" t="s">
+      <c r="C13" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="D13" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="88" t="s">
+      <c r="F13" s="78"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="88" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="87" t="s">
+      <c r="E14" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="F14" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="88" t="s">
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="88"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="87" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="88" t="s">
+      <c r="E15" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="F15" s="78"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="88" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="88"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="87" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="88" t="s">
+      <c r="E16" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="78"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="88" t="s">
+      <c r="C17" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="88" t="s">
+      <c r="D17" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="88"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="87" t="s">
+      <c r="E17" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="F17" s="78"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="88" t="s">
+      <c r="C18" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="88"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="87" t="s">
+      <c r="D18" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="F18" s="78"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="88" t="s">
+      <c r="C19" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="88"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
+      <c r="D19" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="78"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3023,10 +3178,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -3039,175 +3194,173 @@
     <col min="7" max="7" width="7.09210526315789" style="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="30"/>
     <col min="9" max="9" width="17.6315789473684" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.26973684210526" style="60" customWidth="1"/>
+    <col min="10" max="10" width="8.26973684210526" style="52" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="58" customFormat="1" spans="1:10">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+    <row r="1" s="31" customFormat="1" spans="1:10">
+      <c r="A1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="32"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="64"/>
-    </row>
-    <row r="2" s="58" customFormat="1" ht="15" customHeight="1" spans="1:11">
+      <c r="H1" s="42"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="56"/>
+    </row>
+    <row r="2" s="31" customFormat="1" ht="15" customHeight="1" spans="1:11">
       <c r="A2" s="33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" s="58" customFormat="1" ht="25.5" customHeight="1" spans="1:11">
+      <c r="H2" s="43"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" s="31" customFormat="1" ht="25.5" customHeight="1" spans="1:11">
       <c r="A3" s="33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" s="58" customFormat="1" ht="18" customHeight="1" spans="1:11">
+      <c r="H3" s="43"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" s="31" customFormat="1" ht="18" customHeight="1" spans="1:11">
       <c r="A4" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="58" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" s="58" customFormat="1" ht="19.5" customHeight="1" spans="1:11">
+      <c r="H4" s="43"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" s="31" customFormat="1" ht="19.5" customHeight="1" spans="1:11">
       <c r="A5" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" s="58" customFormat="1" ht="15" customHeight="1" spans="1:10">
+      <c r="J5" s="57"/>
+      <c r="K5" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" s="31" customFormat="1" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="37">
-        <f>COUNTIF(G10:G995,"Pass")</f>
-        <v>0</v>
+        <f>COUNTIF(G9:G995,"Pass")</f>
+        <v>7</v>
       </c>
       <c r="B6" s="37">
-        <f>COUNTIF(G10:G995,"Fail")</f>
-        <v>0</v>
+        <f>COUNTIF(G9:G995,"Fail")</f>
+        <v>1</v>
       </c>
       <c r="C6" s="37">
         <f>E6-D6-B6-A6</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="37">
-        <f>COUNTIF(G$10:G$995,"N/A")</f>
+        <f>COUNTIF(G$9:G$995,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="47">
-        <f>COUNTA(A10:A995)</f>
-        <v>4</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="E6" s="44">
+        <f>COUNTA(A9:A995)</f>
+        <v>8</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="65"/>
-    </row>
-    <row r="7" s="58" customFormat="1" ht="15" customHeight="1" spans="4:10">
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" s="31" customFormat="1" ht="15" customHeight="1" spans="4:10">
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="65"/>
-    </row>
-    <row r="8" s="58" customFormat="1" ht="25.5" customHeight="1" spans="1:10">
-      <c r="A8" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="63" t="s">
+      <c r="J7" s="57"/>
+    </row>
+    <row r="8" s="31" customFormat="1" ht="25.5" customHeight="1" spans="1:10">
+      <c r="A8" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="B8" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="C8" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="D8" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="E8" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="F8" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="63" t="s">
+      <c r="H8" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="66"/>
-    </row>
-    <row r="9" s="58" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="I8" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="58"/>
+    </row>
+    <row r="9" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
       <c r="A9" s="40"/>
       <c r="B9" s="40" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -3216,36 +3369,38 @@
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
-      <c r="J9" s="67"/>
-    </row>
-    <row r="10" s="59" customFormat="1" ht="121" customHeight="1" spans="1:10">
+      <c r="J9" s="49"/>
+    </row>
+    <row r="10" ht="96" spans="1:10">
       <c r="A10" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="41"/>
+      <c r="F10" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="68"/>
-    </row>
-    <row r="11" s="58" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="G10" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
       <c r="A11" s="40"/>
       <c r="B11" s="40" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
@@ -3254,28 +3409,38 @@
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" s="40"/>
-      <c r="J11" s="67"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11" s="49"/>
+    </row>
+    <row r="12" ht="36" spans="1:10">
       <c r="A12" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="C12" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>84</v>
+      </c>
       <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="68"/>
-    </row>
-    <row r="13" s="58" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="F12" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
       <c r="A13" s="40"/>
       <c r="B13" s="40" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -3284,39 +3449,243 @@
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" s="40"/>
-      <c r="J13" s="67"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="50" customHeight="1" spans="1:10">
       <c r="A14" s="41" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="68"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="68"/>
+      <c r="C14" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+    </row>
+    <row r="15" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="49"/>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="60" spans="1:10">
+      <c r="A16" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="49"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="84" spans="1:10">
+      <c r="A18" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="49"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="36" spans="1:10">
+      <c r="A20" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+    </row>
+    <row r="21" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="48" spans="1:10">
+      <c r="A22" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
+    </row>
+    <row r="23" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="49"/>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="72" spans="1:10">
+      <c r="A24" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I24" s="50"/>
+      <c r="J24" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3327,11 +3696,11 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G9 G16:G142">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G12 G13 G14 G20 G21 G22 G23 G24 G9:G11 G15:G16 G17:G19">
+      <formula1>$K$2:$K$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G8 G25:G142">
       <formula1>$K$2:$K$6</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G10:G15">
-      <formula1>$K$2:$K$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="1.14930555555556" header="0.511805555555556" footer="0.984027777777778"/>
@@ -3347,10 +3716,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -3376,82 +3745,80 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" s="30" customFormat="1" ht="15" customHeight="1" spans="1:11">
       <c r="A2" s="33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
       <c r="K2" s="30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" s="30" customFormat="1" spans="1:11">
       <c r="A3" s="33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" s="30" customFormat="1" ht="18" customHeight="1" spans="1:11">
       <c r="A4" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>89</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" s="30" customFormat="1" ht="19.5" customHeight="1" spans="1:11">
       <c r="A5" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
@@ -3459,32 +3826,32 @@
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
       <c r="K5" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" s="30" customFormat="1" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="37">
-        <f>COUNTIF(G10:G998,"Pass")</f>
-        <v>0</v>
+        <f>COUNTIF(G9:G996,"Pass")</f>
+        <v>7</v>
       </c>
       <c r="B6" s="37">
-        <f>COUNTIF(G10:G998,"Fail")</f>
+        <f>COUNTIF(G9:G996,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C6" s="37">
         <f>E6-D6-B6-A6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="37">
-        <f>COUNTIF(G$10:G$998,"N/A")</f>
+        <f>COUNTIF(G$9:G$996,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="47">
-        <f>COUNTA(A10:A998)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="E6" s="44">
+        <f>COUNTA(A9:A996)</f>
+        <v>7</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -3500,38 +3867,38 @@
     </row>
     <row r="8" s="30" customFormat="1" ht="25.5" customHeight="1" spans="1:10">
       <c r="A8" s="39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="F8" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="45" t="s">
         <v>72</v>
       </c>
+      <c r="H8" s="45" t="s">
+        <v>73</v>
+      </c>
       <c r="I8" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="54"/>
-    </row>
-    <row r="9" s="30" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+        <v>74</v>
+      </c>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
       <c r="A9" s="40"/>
       <c r="B9" s="40" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -3540,56 +3907,82 @@
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
-      <c r="J9" s="55"/>
-    </row>
-    <row r="10" s="31" customFormat="1" ht="121" customHeight="1" spans="1:10">
+      <c r="J9" s="49"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="36" spans="1:10">
       <c r="A10" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="57"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="41"/>
+      <c r="G10" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="49"/>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="48" spans="1:10">
+      <c r="A12" s="41" t="s">
+        <v>129</v>
+      </c>
       <c r="B12" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
-    </row>
-    <row r="13" s="30" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+        <v>86</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
       <c r="A13" s="40"/>
       <c r="B13" s="40" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -3598,45 +3991,197 @@
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" s="40"/>
-      <c r="J13" s="55"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="41"/>
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="48" spans="1:10">
+      <c r="A14" s="41" t="s">
+        <v>133</v>
+      </c>
       <c r="B14" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+        <v>134</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>136</v>
+      </c>
       <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="7:12">
-      <c r="G16" s="51"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-    </row>
-    <row r="17" spans="7:10">
-      <c r="G17" s="52"/>
-      <c r="J17" s="57"/>
+      <c r="F14" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+    </row>
+    <row r="15" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="49"/>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="60" spans="1:10">
+      <c r="A16" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="49"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="48" spans="1:10">
+      <c r="A18" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="49"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="48" spans="1:10">
+      <c r="A20" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+    </row>
+    <row r="21" s="31" customFormat="1" ht="15.75" customHeight="1" spans="1:10">
+      <c r="A21" s="40"/>
+      <c r="B21" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="72" spans="1:10">
+      <c r="A22" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="46">
+        <v>44645</v>
+      </c>
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3646,8 +4191,11 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G9 G10:G15 G16:G144">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G9 G10 G11 G12 G13 G14 G15 G16 G17:G18 G19:G20 G21:G22">
+      <formula1>$K$2:$K$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G8 G23:G142">
       <formula1>$K$2:$K$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3667,7 +4215,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="7"/>
@@ -3682,7 +4230,7 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1" spans="2:8">
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3710,7 +4258,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="24" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="25"/>
@@ -3719,7 +4267,7 @@
     <row r="4" ht="21.75" customHeight="1" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="7" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3763,22 +4311,22 @@
         <v>11</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3792,15 +4340,15 @@
       </c>
       <c r="D9" s="15">
         <f>Admin!A6</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E9" s="15">
         <f>Admin!B6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="15">
         <f>Admin!C6</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="15">
         <f>Admin!D6</f>
@@ -3808,7 +4356,7 @@
       </c>
       <c r="H9" s="15">
         <f>Admin!E6</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3822,7 +4370,7 @@
       </c>
       <c r="D10" s="15">
         <f>Participant!A6</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E10" s="15">
         <f>Participant!B6</f>
@@ -3830,7 +4378,7 @@
       </c>
       <c r="F10" s="15">
         <f>Participant!C6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="15">
         <f>Participant!D6</f>
@@ -3838,7 +4386,7 @@
       </c>
       <c r="H10" s="15">
         <f>Participant!E6</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3855,19 +4403,19 @@
       <c r="A12" s="11"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="D12" s="19">
         <f>SUM(D7:D11)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E12" s="19">
         <f>SUM(E7:E11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="19">
         <f>SUM(F7:F11)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="19">
         <f>SUM(G7:G11)</f>
@@ -3875,7 +4423,7 @@
       </c>
       <c r="H12" s="19">
         <f>SUM(H7:H11)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3892,15 +4440,15 @@
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="22" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="28">
         <f>(D12+E12)*100/(H12-G12)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="29"/>
@@ -3909,15 +4457,15 @@
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="22" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="28">
         <f>D12*100/(H12-G12)</f>
-        <v>0</v>
+        <v>93.3333333333333</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="29"/>

</xml_diff>

<commit_message>
feat: update test result
</commit_message>
<xml_diff>
--- a/documents/BDP305x_TestCases_template.xlsx
+++ b/documents/BDP305x_TestCases_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="14140" tabRatio="821" activeTab="1"/>
+    <workbookView windowWidth="28000" windowHeight="14140" tabRatio="821" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -628,10 +628,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="d\-mmm\-yy;@"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="d\-mmm\-yy;@"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="42">
@@ -770,13 +770,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -807,9 +800,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -822,49 +814,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -883,10 +837,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -898,8 +889,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -911,15 +919,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,13 +988,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,25 +1042,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,37 +1084,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,7 +1102,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,61 +1144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,7 +1156,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,46 +1454,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1514,6 +1479,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1527,168 +1518,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1698,11 +1698,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1733,7 +1733,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1936,26 +1936,26 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="47" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="19" xfId="47" applyFill="1" applyBorder="1"/>
@@ -1970,10 +1970,10 @@
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2 23" xfId="2"/>
-    <cellStyle name="Normal_Functional Test Case v1.0" xfId="3"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="4"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="1"/>
+    <cellStyle name="Normal_Functional Test Case v1.0" xfId="2"/>
+    <cellStyle name="Normal 2 2 23" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="6" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="7" builtinId="48"/>
@@ -2867,7 +2867,7 @@
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="E30:G30"/>
   </mergeCells>
-  <pageMargins left="0.470138888888889" right="0.470138888888889" top="0.5" bottom="0.35" header="0.511805555555556" footer="0.170138888888889"/>
+  <pageMargins left="0.470138888888889" right="0.470138888888889" top="0.5" bottom="0.349305555555556" header="0.511805555555556" footer="0.170138888888889"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v2/0&amp;C&amp;"Tahoma,Regular"&amp;8Internal use&amp;R&amp;"tahomaTahoma,Regular"&amp;8&amp;P/&amp;N</oddFooter>
@@ -2880,7 +2880,7 @@
   <sheetPr/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -3180,8 +3180,8 @@
   <sheetPr/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -3294,11 +3294,11 @@
     <row r="6" s="31" customFormat="1" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="37">
         <f>COUNTIF(G9:G995,"Pass")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="37">
         <f>COUNTIF(G9:G995,"Fail")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="37">
         <f>E6-D6-B6-A6</f>
@@ -3559,7 +3559,7 @@
         <v>105</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H18" s="46">
         <v>44645</v>
@@ -3696,7 +3696,7 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G12 G13 G14 G20 G21 G22 G23 G24 G9:G11 G15:G16 G17:G19">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G12 G13 G14 G17 G18 G19 G20 G21 G22 G23 G24 G9:G11 G15:G16">
       <formula1>$K$2:$K$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G8 G25:G142">
@@ -4340,11 +4340,11 @@
       </c>
       <c r="D9" s="15">
         <f>Admin!A6</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="15">
         <f>Admin!B6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="15">
         <f>Admin!C6</f>
@@ -4407,11 +4407,11 @@
       </c>
       <c r="D12" s="19">
         <f>SUM(D7:D11)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="19">
         <f>SUM(E7:E11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="19">
         <f>SUM(F7:F11)</f>
@@ -4462,7 +4462,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="28">
         <f>D12*100/(H12-G12)</f>
-        <v>93.3333333333333</v>
+        <v>100</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>164</v>

</xml_diff>